<commit_message>
Main page, filter function, delete function
</commit_message>
<xml_diff>
--- a/Documentation/ProjectDocumentation/Time_recording.xlsx
+++ b/Documentation/ProjectDocumentation/Time_recording.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1675" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1677" uniqueCount="141">
   <si>
     <t>Nr</t>
   </si>
@@ -449,7 +449,10 @@
     <t>ActionBar, Main page, http call to musicpieces</t>
   </si>
   <si>
-    <t>Main page, Test-Daten</t>
+    <t>Main page, Sortierfunktion, Test-Daten</t>
+  </si>
+  <si>
+    <t>Main page, Filter funktion, Lösch-Funktion</t>
   </si>
 </sst>
 </file>
@@ -3038,7 +3041,7 @@
       </c>
       <c r="AF16" s="81">
         <f>AD17-AE16</f>
-        <v>-43</v>
+        <v>-41</v>
       </c>
     </row>
     <row r="17" spans="2:32" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -3086,7 +3089,7 @@
       </c>
       <c r="R17" s="32">
         <f>'Std-B'!C100</f>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="S17" s="32">
         <f>'Std-B'!C111</f>
@@ -3134,7 +3137,7 @@
       </c>
       <c r="AD17" s="33">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="AE17" s="69"/>
       <c r="AF17" s="82"/>
@@ -3184,7 +3187,7 @@
       </c>
       <c r="R18" s="29">
         <f t="shared" si="6"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="S18" s="29">
         <f t="shared" si="6"/>
@@ -3232,7 +3235,7 @@
       </c>
       <c r="AD18" s="31">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="AE18" s="70"/>
       <c r="AF18" s="156"/>
@@ -7590,7 +7593,7 @@
   <dimension ref="A1:E223"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="E97" sqref="E97"/>
+      <selection activeCell="B99" sqref="B99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8824,7 +8827,7 @@
         <v>135</v>
       </c>
       <c r="C97" s="43">
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="D97" s="46" t="s">
         <v>17</v>
@@ -8837,12 +8840,18 @@
       <c r="A98" s="46">
         <v>5</v>
       </c>
-      <c r="B98" s="42"/>
-      <c r="C98" s="43"/>
+      <c r="B98" s="42" t="s">
+        <v>135</v>
+      </c>
+      <c r="C98" s="43">
+        <v>60</v>
+      </c>
       <c r="D98" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="E98" s="42"/>
+      <c r="E98" s="42" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="99" spans="1:5" s="47" customFormat="1" ht="26.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A99" s="48">
@@ -8862,7 +8871,7 @@
       <c r="B100" s="164"/>
       <c r="C100" s="25">
         <f>ROUND((SUM(C94:C99)/60),0)</f>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D100" s="163" t="s">
         <v>18</v>

</xml_diff>